<commit_message>
results with all iterations
</commit_message>
<xml_diff>
--- a/results/by_outcome/full_results_education_PGI_Brothers_MI.xlsx
+++ b/results/by_outcome/full_results_education_PGI_Brothers_MI.xlsx
@@ -483,10 +483,10 @@
         <v>#NUM!</v>
       </c>
       <c r="H2" t="n">
-        <v>0.593271778237796</v>
+        <v>0.590090404453821</v>
       </c>
       <c r="I2" t="n">
-        <v>0.291783304323464</v>
+        <v>0.295582270908201</v>
       </c>
       <c r="J2" t="e">
         <v>#NUM!</v>
@@ -504,7 +504,7 @@
         <v>#NUM!</v>
       </c>
       <c r="O2" t="n">
-        <v>0.406999065746421</v>
+        <v>0.410178944660381</v>
       </c>
     </row>
     <row r="3">
@@ -524,10 +524,10 @@
         <v>#NUM!</v>
       </c>
       <c r="F3" t="n">
-        <v>0.580794523478386</v>
+        <v>0.581023631753013</v>
       </c>
       <c r="G3" t="n">
-        <v>0.315029186783785</v>
+        <v>0.315306377745138</v>
       </c>
       <c r="H3" t="e">
         <v>#NUM!</v>
@@ -562,13 +562,13 @@
         <v>18</v>
       </c>
       <c r="C4" t="n">
-        <v>0.604924804778172</v>
+        <v>0.60493272865191</v>
       </c>
       <c r="D4" t="n">
-        <v>0.395531930183655</v>
+        <v>0.395523933953698</v>
       </c>
       <c r="E4" t="n">
-        <v>1.00045673496183</v>
+        <v>1.00045666260561</v>
       </c>
       <c r="F4" t="e">
         <v>#NUM!</v>
@@ -583,19 +583,19 @@
         <v>#NUM!</v>
       </c>
       <c r="J4" t="n">
-        <v>0.395351359452848</v>
+        <v>0.395343395207135</v>
       </c>
       <c r="K4" t="n">
-        <v>0.314885367709891</v>
+        <v>0.315162454701054</v>
       </c>
       <c r="L4" t="n">
-        <v>-0.0124715588541878</v>
+        <v>-0.0090626340726711</v>
       </c>
       <c r="M4" t="n">
-        <v>0.0116477062935724</v>
+        <v>0.0148355494532462</v>
       </c>
       <c r="N4" t="n">
-        <v>0.302413808855703</v>
+        <v>0.306099820628382</v>
       </c>
       <c r="O4" t="e">
         <v>#NUM!</v>
@@ -640,13 +640,13 @@
         <v>15</v>
       </c>
       <c r="C2" t="n">
-        <v>0.395351359452848</v>
+        <v>0.395343395207135</v>
       </c>
       <c r="D2" t="n">
-        <v>0.327188036284114</v>
+        <v>0.327346032413468</v>
       </c>
       <c r="E2" t="n">
-        <v>0.463514682621583</v>
+        <v>0.463340758000802</v>
       </c>
     </row>
     <row r="3">
@@ -657,13 +657,13 @@
         <v>15</v>
       </c>
       <c r="C3" t="n">
-        <v>0.302413808855703</v>
+        <v>0.306099820628382</v>
       </c>
       <c r="D3" t="n">
-        <v>0.228707366385173</v>
+        <v>0.23252778120793</v>
       </c>
       <c r="E3" t="n">
-        <v>0.376120251326232</v>
+        <v>0.379671860048835</v>
       </c>
     </row>
     <row r="4">
@@ -674,13 +674,13 @@
         <v>15</v>
       </c>
       <c r="C4" t="n">
-        <v>0.406999065746421</v>
+        <v>0.410178944660381</v>
       </c>
       <c r="D4" t="n">
-        <v>0.335970487190677</v>
+        <v>0.338858924177425</v>
       </c>
       <c r="E4" t="n">
-        <v>0.478027644302165</v>
+        <v>0.481498965143336</v>
       </c>
     </row>
   </sheetData>

</xml_diff>